<commit_message>
a few small changes
</commit_message>
<xml_diff>
--- a/src/test/java/MonthlyExpenses2020test.xlsx
+++ b/src/test/java/MonthlyExpenses2020test.xlsx
@@ -982,21 +982,21 @@
         <v>2761.5299999999997</v>
       </c>
       <c r="D3" s="10" t="n">
-        <f>-27 -79.29 -27 -79.29 -79.29</f>
-        <v>-291.87000000000006</v>
+        <f>-27 -79.29 -27 -79.29 -79.29 -79.29</f>
+        <v>-371.1600000000001</v>
       </c>
       <c r="E3" s="11" t="n">
         <f>-79.29 -27 -27</f>
         <v>-133.29000000000002</v>
       </c>
       <c r="F3" s="10" t="n">
-        <f>-40.94 -79.29 -79.29 -40.94 -79.29 -40.94 -79.29 -40.94 -74.07 -79.29 -27 -40.94 -27 -79.29 -40.94</f>
-        <v>-849.45</v>
+        <f>-40.94 -79.29 -79.29 -40.94 -79.29 -40.94 -79.29 -40.94 -74.07 -79.29 -27 -40.94 -27 -79.29 -40.94 -27.00 -74.07</f>
+        <v>-950.52</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="11" t="n">
-        <f>-79.29 -74.07 -40.94 -27 -27 -27 -74.07 -79.29 -74.07 -40.94 -74.07</f>
-        <v>-617.74</v>
+        <f>-79.29 -74.07 -40.94 -27 -27 -27 -74.07 -79.29 -74.07 -40.94 -74.07 -40.94</f>
+        <v>-658.6800000000001</v>
       </c>
       <c r="I3" s="10" t="n">
         <f>-74.07 -74.07 -74.07 -74.07 -40.94 -74.07 -74.07 -79.29 -74.07 -40.94 -27.00</f>
@@ -1005,7 +1005,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10" t="n">
         <f t="shared" ref="K3:K13" si="1">(B3+C3)+SUM(D3:J3)</f>
-        <v>-112.78000000000065</v>
+        <v>-334.08000000000084</v>
       </c>
       <c r="L3" s="12" t="str">
         <f t="shared" ref="L3:L13" si="2">IF(K3&gt;=1, "Underbudget", "Overbudget")</f>
@@ -1013,11 +1013,11 @@
       </c>
       <c r="M3" s="13" t="n">
         <f t="shared" si="0"/>
-        <v>-0.04536185308680238</v>
+        <v>-0.13437212164602666</v>
       </c>
       <c r="N3" s="14" t="n">
         <f>SUM(D3:J3) + B3</f>
-        <v>-2874.3100000000004</v>
+        <v>-3095.6100000000006</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1037,26 +1037,26 @@
         <v>-1443.07</v>
       </c>
       <c r="E4" s="10" t="n">
-        <f>-67.84 -297.51 -67.84 -67.84 -67.84 -21.89 -39.84 -67.84 -21.89 -67.84 -21.89 -21.89 -39.84</f>
-        <v>-871.7900000000002</v>
+        <f>-67.84 -297.51 -67.84 -67.84 -67.84 -21.89 -39.84 -67.84 -21.89 -67.84 -21.89 -21.89 -39.84 -67.84</f>
+        <v>-939.6300000000002</v>
       </c>
       <c r="F4" s="10" t="n">
-        <f>-39.84 -21.89 -297.51 -67.84 -21.89 -39.84 -297.51 -39.84 -297.51 -297.51</f>
-        <v>-1421.18</v>
+        <f>-39.84 -21.89 -297.51 -67.84 -21.89 -39.84 -297.51 -39.84 -297.51 -297.51 -21.89</f>
+        <v>-1443.0700000000002</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="n">
-        <f>-67.84 -297.51 -297.51 -67.84 -67.84</f>
-        <v>-798.5400000000001</v>
+        <f>-67.84 -297.51 -297.51 -67.84 -67.84 -297.51</f>
+        <v>-1096.0500000000002</v>
       </c>
       <c r="I4" s="10" t="n">
-        <f>-21.89 -297.51</f>
-        <v>-319.4</v>
+        <f>-21.89 -297.51 -39.84</f>
+        <v>-359.24</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10" t="n">
         <f t="shared" si="1"/>
-        <v>-2881.0499999999993</v>
+        <v>-3308.13</v>
       </c>
       <c r="L4" s="12" t="str">
         <f t="shared" si="2"/>
@@ -1064,11 +1064,11 @@
       </c>
       <c r="M4" s="13" t="n">
         <f t="shared" si="0"/>
-        <v>-1.4602900254950755</v>
+        <v>-1.6767599458673141</v>
       </c>
       <c r="N4" s="14" t="n">
         <f t="shared" ref="N4:N13" si="3">SUM(D4:J4)</f>
-        <v>-4853.98</v>
+        <v>-5281.06</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1406,15 +1406,15 @@
       </c>
       <c r="D15" s="17" t="n">
         <f t="shared" ref="D15:K15" si="4">AVERAGE(D2:D13)</f>
-        <v>-867.47</v>
+        <v>-907.115</v>
       </c>
       <c r="E15" s="17" t="n">
         <f>AVERAGE(E2:E14)</f>
-        <v>-502.5400000000001</v>
+        <v>-536.4600000000002</v>
       </c>
       <c r="F15" s="17" t="n">
         <f t="shared" si="4"/>
-        <v>-2404.3757142857144</v>
+        <v>-2421.941428571429</v>
       </c>
       <c r="G15" s="17" t="n">
         <f t="shared" si="4"/>
@@ -1422,11 +1422,11 @@
       </c>
       <c r="H15" s="17" t="n">
         <f>AVERAGE(H2:H14)</f>
-        <v>-708.1400000000001</v>
+        <v>-877.3650000000001</v>
       </c>
       <c r="I15" s="17" t="n">
         <f t="shared" si="4"/>
-        <v>-128.2575</v>
+        <v>-133.2375</v>
       </c>
       <c r="J15" s="17" t="e">
         <f t="shared" si="4"/>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="K15" s="17" t="n">
         <f t="shared" si="4"/>
-        <v>-975.9458333333333</v>
+        <v>-1029.9775000000002</v>
       </c>
       <c r="M15" s="13"/>
     </row>
@@ -1466,15 +1466,15 @@
       </c>
       <c r="D17" s="17" t="n">
         <f t="shared" ref="D17:K17" si="5">SUM(D2:D13)</f>
-        <v>-1734.94</v>
+        <v>-1814.23</v>
       </c>
       <c r="E17" s="17" t="n">
         <f>SUM(E2:E14)</f>
-        <v>-1005.0800000000002</v>
+        <v>-1072.9200000000003</v>
       </c>
       <c r="F17" s="17" t="n">
         <f t="shared" si="5"/>
-        <v>-16830.63</v>
+        <v>-16953.59</v>
       </c>
       <c r="G17" s="17" t="n">
         <f t="shared" si="5"/>
@@ -1482,11 +1482,11 @@
       </c>
       <c r="H17" s="17" t="n">
         <f>SUM(H2:H14)</f>
-        <v>-1416.2800000000002</v>
+        <v>-1754.7300000000002</v>
       </c>
       <c r="I17" s="17" t="n">
         <f t="shared" si="5"/>
-        <v>-1026.06</v>
+        <v>-1065.9</v>
       </c>
       <c r="J17" s="17" t="n">
         <f t="shared" si="5"/>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="K17" s="17" t="n">
         <f t="shared" si="5"/>
-        <v>-11711.35</v>
+        <v>-12359.730000000001</v>
       </c>
       <c r="M17" s="13"/>
     </row>

</xml_diff>